<commit_message>
Minor Updates to Output
</commit_message>
<xml_diff>
--- a/Data/Crosswalk_Habitat_Attributes_and_Actions.xlsx
+++ b/Data/Crosswalk_Habitat_Attributes_and_Actions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CC8FD7-6FB4-42DD-B669-1A6CFDA2D758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EB76F8-7BD9-40D1-B688-EBA128460F6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="15912" windowHeight="11412" xr2:uid="{290B77C2-D905-4BDA-AAC5-A66439709522}"/>
+    <workbookView xWindow="456" yWindow="1236" windowWidth="22044" windowHeight="10284" xr2:uid="{290B77C2-D905-4BDA-AAC5-A66439709522}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,9 +234,6 @@
     <t>Harassment Management</t>
   </si>
   <si>
-    <t>Instream Flow Acquisition, Protection, Restoration</t>
-  </si>
-  <si>
     <t>Reduce dewatering of riparian areas</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>Temperature- Rearing</t>
   </si>
   <si>
-    <t>Side Channel/Off-Channel Habitat Restoration</t>
-  </si>
-  <si>
     <t>Off-Channel- Side-Channels</t>
   </si>
   <si>
@@ -330,7 +324,13 @@
     <t>Entrainment/Stranding</t>
   </si>
   <si>
-    <t>Entrainment/Stranding Mitigation</t>
+    <t>Instream Flow Enhancement</t>
+  </si>
+  <si>
+    <t>Side Channel and Off-Channel Habitat Restoration</t>
+  </si>
+  <si>
+    <t>Entrainment and Stranding Mitigation</t>
   </si>
 </sst>
 </file>
@@ -824,15 +824,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E263BE8E-B697-498A-86E6-DFAF7677C733}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G79" workbookViewId="0">
-      <selection activeCell="R84" sqref="R84"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="55.88671875" customWidth="1"/>
     <col min="4" max="4" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -847,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -926,7 +926,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="4"/>
@@ -1004,11 +1004,11 @@
         <v>10</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F11" s="11"/>
     </row>
@@ -1017,10 +1017,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
@@ -1098,11 +1098,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F17" s="11"/>
     </row>
@@ -1162,11 +1162,11 @@
         <v>23</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F21" s="4"/>
     </row>
@@ -1175,14 +1175,14 @@
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="4"/>
     </row>
@@ -1238,11 +1238,11 @@
         <v>13</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F26" s="4"/>
     </row>
@@ -1286,20 +1286,20 @@
         <v>26</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>97</v>
@@ -1362,11 +1362,11 @@
         <v>38</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F34" s="4"/>
     </row>
@@ -1394,7 +1394,7 @@
         <v>40</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="6"/>
@@ -1408,11 +1408,11 @@
         <v>40</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F37" s="4"/>
     </row>
@@ -1511,10 +1511,10 @@
         <v>22</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="15"/>
@@ -1640,15 +1640,15 @@
         <v>31</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>5</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>31</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="6" t="s">
@@ -1704,15 +1704,15 @@
         <v>33</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>5</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>33</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="6" t="s">
@@ -1768,11 +1768,11 @@
         <v>16</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F60" s="4"/>
     </row>
@@ -1784,13 +1784,13 @@
         <v>16</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="13"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>9</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D62" s="10"/>
       <c r="E62" s="13" t="s">
@@ -1830,11 +1830,11 @@
         <v>59</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F64" s="11"/>
     </row>
@@ -1846,13 +1846,13 @@
         <v>59</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
     </row>
-    <row r="66" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>9</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>59</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="11" t="s">
@@ -1892,11 +1892,11 @@
         <v>60</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D68" s="11"/>
       <c r="E68" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F68" s="11"/>
     </row>
@@ -1908,13 +1908,13 @@
         <v>60</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
     </row>
-    <row r="70" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
         <v>9</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>60</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D70" s="10"/>
       <c r="E70" s="11" t="s">
@@ -1954,11 +1954,11 @@
         <v>61</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D72" s="11"/>
       <c r="E72" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F72" s="11"/>
     </row>
@@ -1970,13 +1970,13 @@
         <v>61</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
     </row>
-    <row r="74" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>9</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>61</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D74" s="10"/>
       <c r="E74" s="11" t="s">
@@ -2064,11 +2064,11 @@
         <v>18</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F79" s="4"/>
     </row>
@@ -2077,10 +2077,10 @@
         <v>5</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D80" s="10"/>
       <c r="E80" s="4"/>
@@ -2091,14 +2091,14 @@
         <v>9</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F81" s="4"/>
     </row>
@@ -2107,14 +2107,14 @@
         <v>5</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F82" s="4"/>
     </row>
@@ -2123,14 +2123,14 @@
         <v>5</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F83" s="4"/>
     </row>
@@ -2139,14 +2139,14 @@
         <v>5</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F84" s="4"/>
     </row>
@@ -2155,14 +2155,14 @@
         <v>5</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F85" s="4"/>
     </row>
@@ -2171,14 +2171,14 @@
         <v>5</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F86" s="4"/>
     </row>
@@ -2187,14 +2187,14 @@
         <v>22</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F87" s="4"/>
     </row>

</xml_diff>